<commit_message>
Fish formatting is faster and more complete
The length-weight calculations are done locally, when possible.
The wide format for Fish data (as presentd by TCRMP) is now part of the program, look for the fish-wide-coded option.
</commit_message>
<xml_diff>
--- a/data/Test_Format_BCG_Wide.xlsx
+++ b/data/Test_Format_BCG_Wide.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS" sheetId="1" state="visible" r:id="rId2"/>
@@ -700,7 +700,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.42"/>
   </cols>
@@ -831,11 +831,11 @@
   </sheetPr>
   <dimension ref="A1:AK5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T4" activeCellId="0" sqref="T4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.57"/>
@@ -1060,8 +1060,14 @@
       <c r="J3" s="0" t="n">
         <v>4015</v>
       </c>
+      <c r="K3" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="L3" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>19</v>
@@ -1113,6 +1119,15 @@
       <c r="J4" s="0" t="n">
         <v>4165</v>
       </c>
+      <c r="K4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="O4" s="0" t="n">
         <v>1</v>
       </c>
@@ -1207,6 +1222,9 @@
       </c>
       <c r="L5" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="O5" s="0" t="n">
         <v>28</v>
@@ -1276,7 +1294,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.69"/>
@@ -1511,11 +1529,11 @@
   </sheetPr>
   <dimension ref="A1:AQ21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z16" activeCellId="0" sqref="Z16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AI5" activeCellId="0" sqref="AI5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.69"/>

</xml_diff>